<commit_message>
[add] instan show data in upload
</commit_message>
<xml_diff>
--- a/src/assets/files/format-create-user.xlsx
+++ b/src/assets/files/format-create-user.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\works\frontend-tnan\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DDoS\Desktop\Coding\Final Project\V1\Demo\dssi-front-end\src\assets\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9722B31E-B04E-4345-A3A8-EF601FF77FD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCCA5FDA-ED2B-4681-AA35-3037978EB831}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{3BFD0E7F-4547-45A1-B6C0-F77DFB4DEAE8}"/>
+    <workbookView xWindow="4725" yWindow="3195" windowWidth="28800" windowHeight="15435" xr2:uid="{3BFD0E7F-4547-45A1-B6C0-F77DFB4DEAE8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="11">
   <si>
     <t>username</t>
   </si>
@@ -56,9 +56,6 @@
     <t>student</t>
   </si>
   <si>
-    <t>ตัวอย่าง</t>
-  </si>
-  <si>
     <t>6111444xxx</t>
   </si>
   <si>
@@ -66,31 +63,37 @@
   </si>
   <si>
     <t>ex.so@ubu.ac.th</t>
+  </si>
+  <si>
+    <t>admin@gm.com</t>
+  </si>
+  <si>
+    <t>Admin ลบตัวอย่างทิ้งด้วยครับ</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Tahoma"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF9C5700"/>
-      <name val="Calibri"/>
+      <name val="Tahoma"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
+      <name val="Tahoma"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -98,7 +101,15 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="Calibri"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Tahoma"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -131,18 +142,21 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="3" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Hyperlink" xfId="3" builtinId="8"/>
-    <cellStyle name="Neutral" xfId="1" builtinId="28"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Warning Text" xfId="2" builtinId="11"/>
+    <cellStyle name="ข้อความเตือน" xfId="2" builtinId="11"/>
+    <cellStyle name="ปกติ" xfId="0" builtinId="0"/>
+    <cellStyle name="ปานกลาง" xfId="1" builtinId="28"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -158,7 +172,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="ธีมของ Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -454,35 +468,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{063A0E77-64C8-4A90-A00E-5DEF18D38860}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="27.140625" customWidth="1"/>
-    <col min="3" max="3" width="27.28515625" customWidth="1"/>
-    <col min="4" max="4" width="11.28515625" customWidth="1"/>
-    <col min="5" max="5" width="18.140625" customWidth="1"/>
+    <col min="2" max="2" width="27.125" customWidth="1"/>
+    <col min="3" max="3" width="27.25" customWidth="1"/>
+    <col min="4" max="4" width="11.25" customWidth="1"/>
+    <col min="5" max="5" width="18.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
       <c r="B1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -490,25 +504,35 @@
         <v>7</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="3"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="3"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E3" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" xr:uid="{F0235CEF-596C-4FC8-A34A-B84CD331EEB5}"/>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{F0235CEF-596C-4FC8-A34A-B84CD331EEB5}"/>
+    <hyperlink ref="D3" r:id="rId2" xr:uid="{4C3166DF-509C-4DDE-8B82-5A038690A7D2}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
@@ -516,7 +540,7 @@
           <x14:formula1>
             <xm:f>Sheet2!$A$1:$A$2</xm:f>
           </x14:formula1>
-          <xm:sqref>D2:D200</xm:sqref>
+          <xm:sqref>C2:C3</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -532,14 +556,14 @@
       <selection sqref="A1:A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>5</v>
       </c>

</xml_diff>